<commit_message>
Updated Excel for Vard och omsorgskontakt.
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/logistics/logistics/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontakt.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/logistics/logistics/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontakt.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="233">
   <si>
     <t>Meddelandestruktur</t>
   </si>
@@ -550,9 +550,6 @@
     <t>documentTime</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>Dokumentets identitet som är unik inom källsystemet</t>
   </si>
   <si>
@@ -572,12 +569,6 @@
   </si>
   <si>
     <t>Författarens HSA-id</t>
-  </si>
-  <si>
-    <t>Sring</t>
-  </si>
-  <si>
-    <t>Kod för författarens befattning. Tillåtna värden från kodverk Befattning (OID 1.2.752.129.2.2.1.4) , se http://www.inera.se/Documents/Infrastrukturtjanster/Katalogtjanst_HSA/Innehll/hsa_innehall_befattning.pdf</t>
   </si>
   <si>
     <t>Författarens namn</t>
@@ -753,6 +744,30 @@
   </si>
   <si>
     <t>Enhetens geografiska plats</t>
+  </si>
+  <si>
+    <t>authorOtherRoleCode</t>
+  </si>
+  <si>
+    <t>Kod för författarens befattning. Tillåtna värden från kodverk Befattning (OID 1.2.752.129.2.2.1.4) , se http://www.inera.se/Documents/Infrastrukturtjanster/Katalogtjanst_HSA/Innehll/hsa_innehall_befattning.pdf. I de fall inte KV Befattning kan användas kan authorOtherRole användas för att ange befattning enligt annat kodverk.</t>
+  </si>
+  <si>
+    <t>authorOtherRoleCodeOID</t>
+  </si>
+  <si>
+    <t>OID för det kodverk som används för författarens befattning</t>
+  </si>
+  <si>
+    <t>authorOtherRole</t>
+  </si>
+  <si>
+    <t>AuthorOtherRoleType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information om författarens befattning om annat kodverk än KV Befattning används </t>
+  </si>
+  <si>
+    <t>Kod för författarens befattning enligt annat kodverk</t>
   </si>
 </sst>
 </file>
@@ -1463,11 +1478,11 @@
   <sheetPr codeName="Blad2">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ151"/>
+  <dimension ref="A1:AZ154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG100" sqref="AG100"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z39" sqref="Y39:Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1604,7 +1619,7 @@
       <c r="U3" s="72"/>
       <c r="V3" s="36"/>
       <c r="W3" s="65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="X3" s="73"/>
       <c r="Y3" s="73"/>
@@ -1692,7 +1707,7 @@
         <v>122</v>
       </c>
       <c r="W5" s="65" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="X5" s="30"/>
       <c r="Y5" s="30"/>
@@ -1701,7 +1716,7 @@
       <c r="AB5" s="30"/>
       <c r="AC5" s="63"/>
       <c r="AD5" s="63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AE5" s="63" t="s">
         <v>95</v>
@@ -2005,7 +2020,7 @@
         <v>153</v>
       </c>
       <c r="W14" s="68" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="X14" s="3"/>
       <c r="Z14" s="3" t="s">
@@ -2013,14 +2028,14 @@
       </c>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AE14" s="3"/>
       <c r="AF14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2092,19 +2107,19 @@
       <c r="V16" s="50"/>
       <c r="W16" s="67"/>
       <c r="Z16" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="AF16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="AG16" s="28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.2">
@@ -2245,7 +2260,7 @@
         <v>139</v>
       </c>
       <c r="W20" s="68" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>163</v>
@@ -2253,14 +2268,14 @@
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AE20" s="3"/>
       <c r="AF20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG20" s="39" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2488,23 +2503,23 @@
       <c r="U27" s="8"/>
       <c r="V27" s="28"/>
       <c r="W27" s="68" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Z27" s="3" t="s">
         <v>97</v>
       </c>
       <c r="AC27" s="3"/>
       <c r="AD27" s="39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AE27" s="39" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AF27" s="3" t="s">
         <v>98</v>
       </c>
       <c r="AG27" s="39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2615,14 +2630,14 @@
       </c>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AE30" s="3"/>
       <c r="AF30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG30" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2693,17 +2708,17 @@
       </c>
       <c r="V32" s="15"/>
       <c r="W32" s="68" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="AA32" s="3" t="s">
         <v>99</v>
       </c>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AE32" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="AF32" s="3" t="s">
         <v>1</v>
@@ -2817,23 +2832,23 @@
         <v>134</v>
       </c>
       <c r="W35" s="68" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="AA35" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3" t="s">
         <v>102</v>
       </c>
       <c r="AE35" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="AF35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AG35" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:34" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -2875,7 +2890,7 @@
       <c r="AF36" s="3"/>
       <c r="AG36" s="49"/>
     </row>
-    <row r="37" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" s="2" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2914,16 +2929,16 @@
       <c r="AB37" s="4"/>
       <c r="AC37" s="5"/>
       <c r="AD37" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE37" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AF37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="AG37" s="39" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="1:34" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2958,7 +2973,7 @@
         <v>158</v>
       </c>
       <c r="W38" s="68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
@@ -2966,14 +2981,12 @@
       <c r="AF38" s="3"/>
       <c r="AG38" s="49"/>
     </row>
-    <row r="39" spans="1:34" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
-      <c r="E39" s="52" t="s">
-        <v>36</v>
-      </c>
+      <c r="E39" s="52"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
@@ -2987,31 +3000,34 @@
       <c r="P39" s="15"/>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
-      <c r="S39" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T39" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="U39" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="V39" s="15"/>
-      <c r="W39" s="67"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="52"/>
+      <c r="W39" s="68"/>
+      <c r="AA39" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="AC39" s="3"/>
-      <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="3"/>
-      <c r="AG39" s="49"/>
-    </row>
-    <row r="40" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD39" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE39" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG39" s="49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
-      <c r="E40" s="52" t="s">
-        <v>29</v>
-      </c>
+      <c r="E40" s="52"/>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
@@ -3025,31 +3041,34 @@
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
       <c r="R40" s="15"/>
-      <c r="S40" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="T40" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U40" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="V40" s="15"/>
-      <c r="W40" s="67"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="52"/>
+      <c r="W40" s="68"/>
+      <c r="AA40" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
-      <c r="AF40" s="3"/>
-      <c r="AG40" s="49"/>
-    </row>
-    <row r="41" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD40" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE40" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="49" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
-      <c r="D41" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="52"/>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -3063,26 +3082,35 @@
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
       <c r="R41" s="15"/>
-      <c r="S41" s="15" t="s">
-        <v>2</v>
-      </c>
+      <c r="S41" s="15"/>
       <c r="T41" s="15"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="67"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="68"/>
+      <c r="AA41" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="AC41" s="3"/>
-      <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="49"/>
-    </row>
-    <row r="42" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD41" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE41" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="49" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
       <c r="E42" s="52" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
@@ -3098,41 +3126,30 @@
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
       <c r="S42" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T42" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U42" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="V42" s="52" t="s">
-        <v>126</v>
-      </c>
-      <c r="W42" s="68" t="s">
-        <v>199</v>
-      </c>
-      <c r="AA42" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="U42" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="V42" s="15"/>
+      <c r="W42" s="67"/>
+      <c r="AA42" s="5"/>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
-      <c r="AE42" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF42" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG42" s="39" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE42" s="3"/>
+      <c r="AG42" s="49"/>
+    </row>
+    <row r="43" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
-      <c r="E43" s="52"/>
+      <c r="E43" s="52" t="s">
+        <v>29</v>
+      </c>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
@@ -3146,36 +3163,31 @@
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="52"/>
-      <c r="W43" s="68"/>
-      <c r="AA43" s="2" t="s">
-        <v>211</v>
-      </c>
+      <c r="S43" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T43" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U43" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="V43" s="15"/>
+      <c r="W43" s="67"/>
       <c r="AC43" s="3"/>
-      <c r="AD43" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE43" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG43" s="49" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:34" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="3"/>
+      <c r="AG43" s="49"/>
+    </row>
+    <row r="44" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
-      <c r="B44" s="28"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E44" s="52"/>
+        <v>14</v>
+      </c>
+      <c r="E44" s="15"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
@@ -3189,34 +3201,27 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
       <c r="R44" s="15"/>
-      <c r="S44" s="58" t="s">
-        <v>1</v>
+      <c r="S44" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="T44" s="15"/>
       <c r="U44" s="10"/>
       <c r="V44" s="15"/>
       <c r="W44" s="67"/>
-      <c r="AA44" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
-      <c r="AE44" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG44" s="49" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="49"/>
+    </row>
+    <row r="45" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
-      <c r="B45" s="28"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
-      <c r="E45" s="52"/>
+      <c r="E45" s="52" t="s">
+        <v>34</v>
+      </c>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
@@ -3230,34 +3235,42 @@
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
-      <c r="S45" s="58"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="67"/>
-      <c r="AA45" s="2" t="s">
-        <v>220</v>
+      <c r="S45" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U45" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="V45" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="W45" s="68" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
       <c r="AE45" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AF45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AG45" s="49" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG45" s="39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
-      <c r="E46" s="52" t="s">
-        <v>3</v>
-      </c>
+      <c r="E46" s="52"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
@@ -3271,43 +3284,37 @@
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
-      <c r="S46" s="58" t="s">
-        <v>1</v>
-      </c>
+      <c r="S46" s="15"/>
       <c r="T46" s="15"/>
-      <c r="U46" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="V46" s="15"/>
-      <c r="W46" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA46" s="3" t="s">
-        <v>176</v>
+      <c r="U46" s="9"/>
+      <c r="V46" s="52"/>
+      <c r="W46" s="68"/>
+      <c r="AA46" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3" t="s">
         <v>102</v>
       </c>
       <c r="AE46" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AF46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AG46" s="39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:34" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG46" s="49" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:34" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
+      <c r="D47" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="E47" s="52"/>
-      <c r="F47" s="52" t="s">
-        <v>27</v>
-      </c>
+      <c r="F47" s="15"/>
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
       <c r="I47" s="15"/>
@@ -3323,31 +3330,32 @@
       <c r="S47" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="T47" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U47" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="V47" s="52" t="s">
-        <v>159</v>
-      </c>
+      <c r="T47" s="15"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="15"/>
       <c r="W47" s="67"/>
+      <c r="AA47" s="2" t="s">
+        <v>211</v>
+      </c>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="3"/>
-      <c r="AG47" s="49"/>
-    </row>
-    <row r="48" spans="1:34" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE47" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="49" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" s="2" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="52"/>
-      <c r="F48" s="52" t="s">
-        <v>26</v>
-      </c>
+      <c r="F48" s="15"/>
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15"/>
@@ -3360,32 +3368,35 @@
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
-      <c r="S48" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T48" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="U48" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="V48" s="52"/>
+      <c r="S48" s="58"/>
+      <c r="T48" s="15"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="15"/>
       <c r="W48" s="67"/>
+      <c r="AA48" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
-      <c r="AE48" s="3"/>
-      <c r="AF48" s="3"/>
-      <c r="AG48" s="49"/>
-    </row>
-    <row r="49" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE48" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG48" s="49" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:34" s="2" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="51" t="s">
-        <v>34</v>
-      </c>
+      <c r="E49" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F49" s="15"/>
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
@@ -3398,38 +3409,42 @@
       <c r="P49" s="15"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
-      <c r="S49" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="T49" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="U49" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="V49" s="52" t="s">
-        <v>160</v>
-      </c>
+      <c r="S49" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T49" s="15"/>
+      <c r="U49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="V49" s="15"/>
       <c r="W49" s="68" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA49" s="3"/>
-      <c r="AB49" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="AA49" s="3" t="s">
+        <v>173</v>
+      </c>
       <c r="AC49" s="3"/>
-      <c r="AD49" s="3"/>
-      <c r="AE49" s="3"/>
-      <c r="AF49" s="3"/>
-      <c r="AG49" s="39"/>
-      <c r="AH49" s="3"/>
-    </row>
-    <row r="50" spans="1:34" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD49" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE49" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
       <c r="E50" s="52"/>
-      <c r="F50" s="15" t="s">
-        <v>44</v>
+      <c r="F50" s="52" t="s">
+        <v>27</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
@@ -3444,31 +3459,32 @@
       <c r="Q50" s="15"/>
       <c r="R50" s="15"/>
       <c r="S50" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T50" s="15" t="s">
         <v>69</v>
       </c>
       <c r="U50" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="V50" s="52"/>
+        <v>66</v>
+      </c>
+      <c r="V50" s="52" t="s">
+        <v>159</v>
+      </c>
       <c r="W50" s="67"/>
-      <c r="AA50" s="3"/>
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
       <c r="AE50" s="3"/>
       <c r="AF50" s="3"/>
       <c r="AG50" s="49"/>
     </row>
-    <row r="51" spans="1:34" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="52"/>
-      <c r="F51" s="15" t="s">
-        <v>45</v>
+      <c r="F51" s="52" t="s">
+        <v>26</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
@@ -3483,37 +3499,30 @@
       <c r="Q51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T51" s="15" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="U51" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="V51" s="52" t="s">
-        <v>161</v>
-      </c>
-      <c r="W51" s="68" t="s">
-        <v>202</v>
-      </c>
-      <c r="AA51" s="3"/>
-      <c r="AB51" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="V51" s="52"/>
+      <c r="W51" s="67"/>
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
       <c r="AE51" s="3"/>
       <c r="AF51" s="3"/>
-      <c r="AG51" s="39"/>
-      <c r="AH51" s="3"/>
-    </row>
-    <row r="52" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG51" s="49"/>
+    </row>
+    <row r="52" spans="1:34" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15" t="s">
-        <v>71</v>
+      <c r="E52" s="52"/>
+      <c r="F52" s="51" t="s">
+        <v>34</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
@@ -3527,31 +3536,40 @@
       <c r="P52" s="15"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
-      <c r="S52" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T52" s="15"/>
-      <c r="U52" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="V52" s="15"/>
-      <c r="W52" s="67"/>
+      <c r="S52" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="T52" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="U52" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="V52" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="W52" s="68" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3"/>
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
       <c r="AE52" s="3"/>
       <c r="AF52" s="3"/>
-      <c r="AG52" s="49"/>
-    </row>
-    <row r="53" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG52" s="39"/>
+      <c r="AH52" s="3"/>
+    </row>
+    <row r="53" spans="1:34" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="E53" s="52"/>
+      <c r="F53" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
@@ -3564,29 +3582,34 @@
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T53" s="15"/>
-      <c r="U53" s="10"/>
-      <c r="V53" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="T53" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U53" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="V53" s="52"/>
       <c r="W53" s="67"/>
+      <c r="AA53" s="3"/>
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
       <c r="AE53" s="3"/>
       <c r="AF53" s="3"/>
       <c r="AG53" s="49"/>
     </row>
-    <row r="54" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" s="2" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="15"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="15" t="s">
-        <v>3</v>
-      </c>
+      <c r="E54" s="52"/>
+      <c r="F54" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -3598,32 +3621,41 @@
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
       <c r="S54" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T54" s="15"/>
-      <c r="U54" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="V54" s="15"/>
-      <c r="W54" s="67"/>
+        <v>2</v>
+      </c>
+      <c r="T54" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U54" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="V54" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="W54" s="68" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="3"/>
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
       <c r="AE54" s="3"/>
       <c r="AF54" s="3"/>
-      <c r="AG54" s="49"/>
-    </row>
-    <row r="55" spans="1:34" s="2" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AG54" s="39"/>
+      <c r="AH54" s="3"/>
+    </row>
+    <row r="55" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
+      <c r="F55" s="15" t="s">
+        <v>71</v>
+      </c>
       <c r="G55" s="15"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
@@ -3636,47 +3668,30 @@
       <c r="S55" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="T55" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U55" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="V55" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="W55" s="68" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA55" s="3" t="s">
-        <v>175</v>
-      </c>
+      <c r="T55" s="15"/>
+      <c r="U55" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="V55" s="15"/>
+      <c r="W55" s="67"/>
       <c r="AC55" s="3"/>
-      <c r="AD55" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE55" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF55" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG55" s="39" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD55" s="3"/>
+      <c r="AE55" s="3"/>
+      <c r="AF55" s="3"/>
+      <c r="AG55" s="49"/>
+    </row>
+    <row r="56" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
-      <c r="G56" s="15"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="G56" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
       <c r="J56" s="15"/>
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
@@ -3686,16 +3701,12 @@
       <c r="P56" s="15"/>
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
-      <c r="S56" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="T56" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="U56" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="V56" s="51"/>
+      <c r="S56" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T56" s="15"/>
+      <c r="U56" s="10"/>
+      <c r="V56" s="15"/>
       <c r="W56" s="67"/>
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
@@ -3703,17 +3714,17 @@
       <c r="AF56" s="3"/>
       <c r="AG56" s="49"/>
     </row>
-    <row r="57" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
-      <c r="B57" s="15" t="s">
-        <v>16</v>
-      </c>
+      <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="15" t="s">
+        <v>3</v>
+      </c>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
       <c r="K57" s="15"/>
@@ -3724,36 +3735,33 @@
       <c r="P57" s="15"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
-      <c r="S57" s="15" t="s">
+      <c r="S57" s="58" t="s">
         <v>1</v>
       </c>
       <c r="T57" s="15"/>
-      <c r="U57" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="V57" s="54"/>
+      <c r="U57" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="V57" s="15"/>
       <c r="W57" s="67"/>
-      <c r="Z57" s="3"/>
-      <c r="AA57" s="3"/>
-      <c r="AB57" s="3"/>
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
       <c r="AE57" s="3"/>
       <c r="AF57" s="3"/>
-      <c r="AG57" s="39"/>
-    </row>
-    <row r="58" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG57" s="49"/>
+    </row>
+    <row r="58" spans="1:34" s="2" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
-      <c r="C58" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="J58" s="15"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
@@ -3763,34 +3771,50 @@
       <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
-      <c r="S58" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T58" s="15"/>
-      <c r="U58" s="8"/>
-      <c r="V58" s="28"/>
-      <c r="W58" s="67"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AB58" s="3"/>
+      <c r="S58" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T58" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U58" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="V58" s="51" t="s">
+        <v>131</v>
+      </c>
+      <c r="W58" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA58" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="3"/>
-      <c r="AG58" s="39"/>
-    </row>
-    <row r="59" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AD58" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE58" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG58" s="39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
-      <c r="D59" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
@@ -3800,30 +3824,31 @@
       <c r="P59" s="15"/>
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
-      <c r="S59" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T59" s="15"/>
-      <c r="U59" s="10"/>
-      <c r="V59" s="15"/>
+      <c r="S59" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="T59" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="U59" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V59" s="51"/>
       <c r="W59" s="67"/>
-      <c r="Z59" s="3"/>
-      <c r="AA59" s="3"/>
-      <c r="AB59" s="3"/>
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
       <c r="AE59" s="3"/>
       <c r="AF59" s="3"/>
-      <c r="AG59" s="39"/>
+      <c r="AG59" s="49"/>
     </row>
     <row r="60" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
+      <c r="B60" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
-      <c r="E60" s="52" t="s">
-        <v>8</v>
-      </c>
+      <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
@@ -3841,10 +3866,10 @@
         <v>1</v>
       </c>
       <c r="T60" s="15"/>
-      <c r="U60" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="V60" s="15"/>
+      <c r="U60" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V60" s="54"/>
       <c r="W60" s="67"/>
       <c r="Z60" s="3"/>
       <c r="AA60" s="3"/>
@@ -3858,12 +3883,12 @@
     <row r="61" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
+      <c r="C61" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="52" t="s">
-        <v>27</v>
-      </c>
+      <c r="F61" s="15"/>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
@@ -3879,15 +3904,9 @@
       <c r="S61" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T61" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U61" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="V61" s="52" t="s">
-        <v>136</v>
-      </c>
+      <c r="T61" s="15"/>
+      <c r="U61" s="8"/>
+      <c r="V61" s="28"/>
       <c r="W61" s="67"/>
       <c r="Z61" s="3"/>
       <c r="AA61" s="3"/>
@@ -3902,11 +3921,11 @@
       <c r="A62" s="15"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
+      <c r="D62" s="15" t="s">
+        <v>18</v>
+      </c>
       <c r="E62" s="15"/>
-      <c r="F62" s="52" t="s">
-        <v>37</v>
-      </c>
+      <c r="F62" s="15"/>
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
@@ -3922,14 +3941,9 @@
       <c r="S62" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T62" s="15" t="str">
-        <f>"1.2.752.129.2.1.4.1"</f>
-        <v>1.2.752.129.2.1.4.1</v>
-      </c>
-      <c r="U62" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="V62" s="51"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="10"/>
+      <c r="V62" s="15"/>
       <c r="W62" s="67"/>
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
@@ -3942,12 +3956,12 @@
     </row>
     <row r="63" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="15" t="s">
-        <v>204</v>
-      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
       <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
+      <c r="E63" s="52" t="s">
+        <v>8</v>
+      </c>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
@@ -3965,11 +3979,11 @@
         <v>1</v>
       </c>
       <c r="T63" s="15"/>
-      <c r="U63" s="10"/>
-      <c r="V63" s="49"/>
+      <c r="U63" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="V63" s="15"/>
       <c r="W63" s="67"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="15"/>
       <c r="Z63" s="3"/>
       <c r="AA63" s="3"/>
       <c r="AB63" s="3"/>
@@ -3981,13 +3995,13 @@
     </row>
     <row r="64" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15"/>
-      <c r="B64" s="28"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="52" t="s">
-        <v>24</v>
-      </c>
+      <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
+      <c r="F64" s="52" t="s">
+        <v>27</v>
+      </c>
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
@@ -4003,14 +4017,16 @@
       <c r="S64" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T64" s="15"/>
+      <c r="T64" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="U64" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="V64" s="49"/>
+        <v>175</v>
+      </c>
+      <c r="V64" s="52" t="s">
+        <v>136</v>
+      </c>
       <c r="W64" s="67"/>
-      <c r="X64" s="52"/>
-      <c r="Y64" s="52"/>
       <c r="Z64" s="3"/>
       <c r="AA64" s="3"/>
       <c r="AB64" s="3"/>
@@ -4020,15 +4036,15 @@
       <c r="AF64" s="3"/>
       <c r="AG64" s="39"/>
     </row>
-    <row r="65" spans="1:52" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15"/>
-      <c r="B65" s="28"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="15"/>
-      <c r="D65" s="28"/>
-      <c r="E65" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="F65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="52" t="s">
+        <v>37</v>
+      </c>
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
       <c r="I65" s="15"/>
@@ -4044,16 +4060,15 @@
       <c r="S65" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T65" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U65" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="V65" s="49"/>
+      <c r="T65" s="15" t="str">
+        <f>"1.2.752.129.2.1.4.1"</f>
+        <v>1.2.752.129.2.1.4.1</v>
+      </c>
+      <c r="U65" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="V65" s="51"/>
       <c r="W65" s="67"/>
-      <c r="X65" s="52"/>
-      <c r="Y65" s="52"/>
       <c r="Z65" s="3"/>
       <c r="AA65" s="3"/>
       <c r="AB65" s="3"/>
@@ -4063,14 +4078,14 @@
       <c r="AF65" s="3"/>
       <c r="AG65" s="39"/>
     </row>
-    <row r="66" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15"/>
       <c r="B66" s="28"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="52" t="s">
-        <v>28</v>
-      </c>
+      <c r="C66" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="H66" s="15"/>
@@ -4087,16 +4102,12 @@
       <c r="S66" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T66" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="U66" s="70" t="s">
-        <v>93</v>
-      </c>
+      <c r="T66" s="15"/>
+      <c r="U66" s="10"/>
       <c r="V66" s="49"/>
       <c r="W66" s="67"/>
-      <c r="X66" s="71"/>
-      <c r="Y66" s="71"/>
+      <c r="X66" s="15"/>
+      <c r="Y66" s="15"/>
       <c r="Z66" s="3"/>
       <c r="AA66" s="3"/>
       <c r="AB66" s="3"/>
@@ -4106,14 +4117,14 @@
       <c r="AF66" s="3"/>
       <c r="AG66" s="39"/>
     </row>
-    <row r="67" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="28"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="52" t="s">
-        <v>207</v>
-      </c>
+      <c r="D67" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" s="15"/>
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
       <c r="H67" s="15"/>
@@ -4127,15 +4138,17 @@
       <c r="P67" s="15"/>
       <c r="Q67" s="15"/>
       <c r="R67" s="15"/>
-      <c r="S67" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T67" s="28"/>
-      <c r="U67" s="8"/>
+      <c r="S67" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T67" s="15"/>
+      <c r="U67" s="9" t="s">
+        <v>202</v>
+      </c>
       <c r="V67" s="49"/>
       <c r="W67" s="67"/>
-      <c r="X67" s="28"/>
-      <c r="Y67" s="28"/>
+      <c r="X67" s="52"/>
+      <c r="Y67" s="52"/>
       <c r="Z67" s="3"/>
       <c r="AA67" s="3"/>
       <c r="AB67" s="3"/>
@@ -4145,15 +4158,15 @@
       <c r="AF67" s="3"/>
       <c r="AG67" s="39"/>
     </row>
-    <row r="68" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:33" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A68" s="15"/>
       <c r="B68" s="28"/>
       <c r="C68" s="15"/>
       <c r="D68" s="28"/>
-      <c r="E68" s="52"/>
-      <c r="F68" s="52" t="s">
-        <v>9</v>
-      </c>
+      <c r="E68" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="15"/>
       <c r="G68" s="15"/>
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
@@ -4166,13 +4179,15 @@
       <c r="P68" s="15"/>
       <c r="Q68" s="15"/>
       <c r="R68" s="15"/>
-      <c r="S68" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="T68" s="51" t="s">
-        <v>208</v>
-      </c>
-      <c r="U68" s="9"/>
+      <c r="S68" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T68" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U68" s="17" t="s">
+        <v>203</v>
+      </c>
       <c r="V68" s="49"/>
       <c r="W68" s="67"/>
       <c r="X68" s="52"/>
@@ -4186,14 +4201,14 @@
       <c r="AF68" s="3"/>
       <c r="AG68" s="39"/>
     </row>
-    <row r="69" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15"/>
-      <c r="B69" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="B69" s="28"/>
       <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="52" t="s">
+        <v>28</v>
+      </c>
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
       <c r="H69" s="15"/>
@@ -4210,20 +4225,33 @@
       <c r="S69" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T69" s="15"/>
-      <c r="U69" s="10"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="68"/>
-      <c r="AG69" s="28"/>
-    </row>
-    <row r="70" spans="1:52" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T69" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="U69" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="V69" s="49"/>
+      <c r="W69" s="67"/>
+      <c r="X69" s="71"/>
+      <c r="Y69" s="71"/>
+      <c r="Z69" s="3"/>
+      <c r="AA69" s="3"/>
+      <c r="AB69" s="3"/>
+      <c r="AC69" s="3"/>
+      <c r="AD69" s="3"/>
+      <c r="AE69" s="3"/>
+      <c r="AF69" s="3"/>
+      <c r="AG69" s="39"/>
+    </row>
+    <row r="70" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="52" t="s">
+        <v>204</v>
+      </c>
       <c r="F70" s="15"/>
       <c r="G70" s="15"/>
       <c r="H70" s="15"/>
@@ -4237,24 +4265,33 @@
       <c r="P70" s="15"/>
       <c r="Q70" s="15"/>
       <c r="R70" s="15"/>
-      <c r="S70" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T70" s="15"/>
-      <c r="U70" s="10"/>
-      <c r="V70" s="15"/>
+      <c r="S70" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T70" s="28"/>
+      <c r="U70" s="8"/>
+      <c r="V70" s="49"/>
       <c r="W70" s="67"/>
-      <c r="AG70" s="15"/>
-    </row>
-    <row r="71" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="28"/>
-      <c r="B71" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="28"/>
+      <c r="X70" s="28"/>
+      <c r="Y70" s="28"/>
+      <c r="Z70" s="3"/>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="3"/>
+      <c r="AC70" s="3"/>
+      <c r="AD70" s="3"/>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="3"/>
+      <c r="AG70" s="39"/>
+    </row>
+    <row r="71" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="15"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="15"/>
       <c r="D71" s="28"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="15"/>
+      <c r="E71" s="52"/>
+      <c r="F71" s="52" t="s">
+        <v>9</v>
+      </c>
       <c r="G71" s="15"/>
       <c r="H71" s="15"/>
       <c r="I71" s="15"/>
@@ -4267,20 +4304,33 @@
       <c r="P71" s="15"/>
       <c r="Q71" s="15"/>
       <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="10"/>
-      <c r="V71" s="15"/>
+      <c r="S71" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T71" s="51" t="s">
+        <v>205</v>
+      </c>
+      <c r="U71" s="9"/>
+      <c r="V71" s="49"/>
       <c r="W71" s="67"/>
-      <c r="AG71" s="28"/>
-    </row>
-    <row r="72" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="28"/>
-      <c r="B72" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
+      <c r="X71" s="52"/>
+      <c r="Y71" s="52"/>
+      <c r="Z71" s="3"/>
+      <c r="AA71" s="3"/>
+      <c r="AB71" s="3"/>
+      <c r="AC71" s="3"/>
+      <c r="AD71" s="3"/>
+      <c r="AE71" s="3"/>
+      <c r="AF71" s="3"/>
+      <c r="AG71" s="39"/>
+    </row>
+    <row r="72" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
       <c r="E72" s="15"/>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
@@ -4295,20 +4345,22 @@
       <c r="P72" s="15"/>
       <c r="Q72" s="15"/>
       <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
+      <c r="S72" s="15" t="s">
+        <v>1</v>
+      </c>
       <c r="T72" s="15"/>
       <c r="U72" s="10"/>
       <c r="V72" s="15"/>
       <c r="W72" s="68"/>
       <c r="AG72" s="28"/>
     </row>
-    <row r="73" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="28"/>
-      <c r="B73" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
+    <row r="73" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -4323,20 +4375,22 @@
       <c r="P73" s="15"/>
       <c r="Q73" s="15"/>
       <c r="R73" s="15"/>
-      <c r="S73" s="15"/>
+      <c r="S73" s="15" t="s">
+        <v>1</v>
+      </c>
       <c r="T73" s="15"/>
       <c r="U73" s="10"/>
       <c r="V73" s="15"/>
       <c r="W73" s="67"/>
-      <c r="AG73" s="28"/>
-    </row>
-    <row r="74" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="AG73" s="15"/>
+    </row>
+    <row r="74" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="28"/>
+      <c r="B74" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
@@ -4351,26 +4405,21 @@
       <c r="P74" s="15"/>
       <c r="Q74" s="15"/>
       <c r="R74" s="15"/>
-      <c r="S74" s="15" t="s">
-        <v>1</v>
-      </c>
+      <c r="S74" s="15"/>
       <c r="T74" s="15"/>
-      <c r="U74" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="U74" s="10"/>
       <c r="V74" s="15"/>
       <c r="W74" s="67"/>
-      <c r="Z74" s="3"/>
       <c r="AG74" s="28"/>
     </row>
-    <row r="75" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="15"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15" t="s">
-        <v>21</v>
-      </c>
+    <row r="75" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="28"/>
+      <c r="B75" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="15"/>
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
       <c r="H75" s="15"/>
@@ -4384,24 +4433,22 @@
       <c r="P75" s="15"/>
       <c r="Q75" s="15"/>
       <c r="R75" s="15"/>
-      <c r="S75" s="15" t="s">
-        <v>1</v>
-      </c>
+      <c r="S75" s="15"/>
       <c r="T75" s="15"/>
       <c r="U75" s="10"/>
       <c r="V75" s="15"/>
-      <c r="W75" s="67"/>
+      <c r="W75" s="68"/>
       <c r="AG75" s="28"/>
     </row>
-    <row r="76" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="15"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
+    <row r="76" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="28"/>
+      <c r="B76" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
       <c r="E76" s="15"/>
-      <c r="F76" s="52" t="s">
-        <v>9</v>
-      </c>
+      <c r="F76" s="15"/>
       <c r="G76" s="15"/>
       <c r="H76" s="15"/>
       <c r="I76" s="15"/>
@@ -4414,29 +4461,23 @@
       <c r="P76" s="15"/>
       <c r="Q76" s="15"/>
       <c r="R76" s="15"/>
-      <c r="S76" s="15" t="s">
-        <v>1</v>
-      </c>
+      <c r="S76" s="15"/>
       <c r="T76" s="15"/>
-      <c r="U76" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="V76" s="53" t="s">
-        <v>141</v>
-      </c>
+      <c r="U76" s="10"/>
+      <c r="V76" s="15"/>
       <c r="W76" s="67"/>
       <c r="AG76" s="28"/>
     </row>
-    <row r="77" spans="1:52" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
+      <c r="D77" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
-      <c r="G77" s="52" t="s">
-        <v>24</v>
-      </c>
+      <c r="G77" s="15"/>
       <c r="H77" s="15"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
@@ -4451,39 +4492,25 @@
       <c r="S77" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T77" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U77" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="V77" s="53"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="V77" s="15"/>
       <c r="W77" s="67"/>
-      <c r="X77" s="3"/>
-      <c r="Z77" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AD77" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE77" s="3"/>
-      <c r="AF77" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG77" s="49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:52" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Z77" s="3"/>
+      <c r="AG77" s="28"/>
+    </row>
+    <row r="78" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
       <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
+      <c r="E78" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="F78" s="15"/>
-      <c r="G78" s="52" t="s">
-        <v>28</v>
-      </c>
+      <c r="G78" s="15"/>
       <c r="H78" s="15"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
@@ -4498,28 +4525,22 @@
       <c r="S78" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T78" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="U78" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="V78" s="54"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="10"/>
+      <c r="V78" s="15"/>
       <c r="W78" s="67"/>
-      <c r="Y78" s="3"/>
-      <c r="Z78" s="25"/>
       <c r="AG78" s="28"/>
     </row>
-    <row r="79" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="15"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
-      <c r="F79" s="52"/>
-      <c r="G79" s="52" t="s">
-        <v>29</v>
-      </c>
+      <c r="F79" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" s="15"/>
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
@@ -4531,30 +4552,29 @@
       <c r="P79" s="15"/>
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
-      <c r="S79" s="52" t="s">
+      <c r="S79" s="15" t="s">
         <v>1</v>
       </c>
       <c r="T79" s="15"/>
-      <c r="U79" s="11"/>
-      <c r="V79" s="53"/>
+      <c r="U79" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="V79" s="53" t="s">
+        <v>141</v>
+      </c>
       <c r="W79" s="67"/>
-      <c r="Y79" s="3"/>
-      <c r="Z79" s="25"/>
       <c r="AG79" s="28"/>
-      <c r="AZ79" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:33" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A80" s="15"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
       <c r="D80" s="15"/>
       <c r="E80" s="15"/>
-      <c r="F80" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G80" s="52"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="52" t="s">
+        <v>24</v>
+      </c>
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
@@ -4566,28 +4586,41 @@
       <c r="P80" s="15"/>
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
-      <c r="S80" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="T80" s="15"/>
+      <c r="S80" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T80" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="U80" s="11" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="V80" s="53"/>
       <c r="W80" s="67"/>
-      <c r="Y80" s="3"/>
-      <c r="Z80" s="25"/>
-      <c r="AG80" s="28"/>
-    </row>
-    <row r="81" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X80" s="3"/>
+      <c r="Z80" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD80" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG80" s="49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:52" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="15"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
-      <c r="F81" s="52"/>
+      <c r="F81" s="15"/>
       <c r="G81" s="52" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="15"/>
@@ -4600,26 +4633,32 @@
       <c r="P81" s="15"/>
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
-      <c r="S81" s="52"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="11"/>
-      <c r="V81" s="53"/>
+      <c r="S81" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T81" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="U81" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="V81" s="54"/>
       <c r="W81" s="67"/>
       <c r="Y81" s="3"/>
       <c r="Z81" s="25"/>
       <c r="AG81" s="28"/>
     </row>
-    <row r="82" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
       <c r="F82" s="52"/>
-      <c r="G82" s="52"/>
-      <c r="H82" s="52" t="s">
-        <v>38</v>
-      </c>
+      <c r="G82" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H82" s="15"/>
       <c r="I82" s="15"/>
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
@@ -4630,28 +4669,31 @@
       <c r="P82" s="15"/>
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
-      <c r="S82" s="52"/>
-      <c r="T82" s="52" t="s">
-        <v>48</v>
-      </c>
+      <c r="S82" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="T82" s="15"/>
       <c r="U82" s="11"/>
       <c r="V82" s="53"/>
-      <c r="W82" s="68"/>
+      <c r="W82" s="67"/>
       <c r="Y82" s="3"/>
       <c r="Z82" s="25"/>
       <c r="AG82" s="28"/>
-    </row>
-    <row r="83" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AZ82" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
-      <c r="F83" s="52"/>
+      <c r="F83" s="52" t="s">
+        <v>22</v>
+      </c>
       <c r="G83" s="52"/>
-      <c r="H83" s="52" t="s">
-        <v>40</v>
-      </c>
+      <c r="H83" s="15"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
       <c r="K83" s="15"/>
@@ -4662,28 +4704,30 @@
       <c r="P83" s="15"/>
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
-      <c r="S83" s="52"/>
-      <c r="T83" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="U83" s="11"/>
+      <c r="S83" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="T83" s="15"/>
+      <c r="U83" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="V83" s="53"/>
       <c r="W83" s="67"/>
       <c r="Y83" s="3"/>
       <c r="Z83" s="25"/>
       <c r="AG83" s="28"/>
     </row>
-    <row r="84" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
       <c r="D84" s="15"/>
       <c r="E84" s="15"/>
       <c r="F84" s="52"/>
-      <c r="G84" s="52"/>
-      <c r="H84" s="52" t="s">
-        <v>24</v>
-      </c>
+      <c r="G84" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="H84" s="15"/>
       <c r="I84" s="15"/>
       <c r="J84" s="15"/>
       <c r="K84" s="15"/>
@@ -4698,12 +4742,12 @@
       <c r="T84" s="15"/>
       <c r="U84" s="11"/>
       <c r="V84" s="53"/>
-      <c r="W84" s="53"/>
+      <c r="W84" s="67"/>
       <c r="Y84" s="3"/>
       <c r="Z84" s="25"/>
       <c r="AG84" s="28"/>
     </row>
-    <row r="85" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="15"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
@@ -4711,10 +4755,10 @@
       <c r="E85" s="15"/>
       <c r="F85" s="52"/>
       <c r="G85" s="52"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="52" t="s">
-        <v>24</v>
-      </c>
+      <c r="H85" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="I85" s="15"/>
       <c r="J85" s="15"/>
       <c r="K85" s="15"/>
       <c r="L85" s="15"/>
@@ -4726,18 +4770,16 @@
       <c r="R85" s="15"/>
       <c r="S85" s="52"/>
       <c r="T85" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="U85" s="11" t="s">
-        <v>116</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="U85" s="11"/>
       <c r="V85" s="53"/>
-      <c r="W85" s="53"/>
+      <c r="W85" s="68"/>
       <c r="Y85" s="3"/>
       <c r="Z85" s="25"/>
       <c r="AG85" s="28"/>
     </row>
-    <row r="86" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
@@ -4745,10 +4787,10 @@
       <c r="E86" s="15"/>
       <c r="F86" s="52"/>
       <c r="G86" s="52"/>
-      <c r="H86" s="15"/>
-      <c r="I86" s="52" t="s">
-        <v>28</v>
-      </c>
+      <c r="H86" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="I86" s="15"/>
       <c r="J86" s="15"/>
       <c r="K86" s="15"/>
       <c r="L86" s="15"/>
@@ -4759,19 +4801,17 @@
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
       <c r="S86" s="52"/>
-      <c r="T86" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="U86" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="T86" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="U86" s="11"/>
       <c r="V86" s="53"/>
-      <c r="W86" s="53"/>
+      <c r="W86" s="67"/>
       <c r="Y86" s="3"/>
       <c r="Z86" s="25"/>
       <c r="AG86" s="28"/>
     </row>
-    <row r="87" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="15"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
@@ -4779,10 +4819,10 @@
       <c r="E87" s="15"/>
       <c r="F87" s="52"/>
       <c r="G87" s="52"/>
-      <c r="H87" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="I87" s="52"/>
+      <c r="H87" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="I87" s="15"/>
       <c r="J87" s="15"/>
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
@@ -4792,34 +4832,16 @@
       <c r="P87" s="15"/>
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
-      <c r="S87" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="T87" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="U87" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="V87" s="53" t="s">
-        <v>150</v>
-      </c>
+      <c r="S87" s="52"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="11"/>
+      <c r="V87" s="53"/>
       <c r="W87" s="53"/>
       <c r="Y87" s="3"/>
-      <c r="Z87" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD87" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF87" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG87" s="62" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="88" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z87" s="25"/>
+      <c r="AG87" s="28"/>
+    </row>
+    <row r="88" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
@@ -4827,10 +4849,10 @@
       <c r="E88" s="15"/>
       <c r="F88" s="52"/>
       <c r="G88" s="52"/>
-      <c r="H88" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="I88" s="52"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="52" t="s">
+        <v>24</v>
+      </c>
       <c r="J88" s="15"/>
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
@@ -4840,33 +4862,20 @@
       <c r="P88" s="15"/>
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
-      <c r="S88" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="T88" s="51"/>
+      <c r="S88" s="52"/>
+      <c r="T88" s="52" t="s">
+        <v>115</v>
+      </c>
       <c r="U88" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="V88" s="53" t="s">
-        <v>113</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="V88" s="53"/>
       <c r="W88" s="53"/>
       <c r="Y88" s="3"/>
-      <c r="Z88" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="AD88" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AE88" s="3"/>
-      <c r="AF88" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG88" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="89" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z88" s="25"/>
+      <c r="AG88" s="28"/>
+    </row>
+    <row r="89" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -4874,10 +4883,10 @@
       <c r="E89" s="15"/>
       <c r="F89" s="52"/>
       <c r="G89" s="52"/>
-      <c r="H89" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="I89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="52" t="s">
+        <v>28</v>
+      </c>
       <c r="J89" s="15"/>
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
@@ -4887,28 +4896,20 @@
       <c r="P89" s="15"/>
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
-      <c r="S89" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="T89" s="15"/>
-      <c r="U89" s="11"/>
+      <c r="S89" s="52"/>
+      <c r="T89" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="U89" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="V89" s="53"/>
       <c r="W89" s="53"/>
       <c r="Y89" s="3"/>
-      <c r="Z89" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE89" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AF89" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG89" s="28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="90" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z89" s="25"/>
+      <c r="AG89" s="28"/>
+    </row>
+    <row r="90" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
@@ -4916,10 +4917,10 @@
       <c r="E90" s="15"/>
       <c r="F90" s="52"/>
       <c r="G90" s="52"/>
-      <c r="H90" s="58"/>
-      <c r="I90" s="52" t="s">
-        <v>111</v>
-      </c>
+      <c r="H90" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="I90" s="52"/>
       <c r="J90" s="15"/>
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
@@ -4930,19 +4931,33 @@
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
       <c r="S90" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="T90" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="U90" s="11"/>
-      <c r="V90" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="T90" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="U90" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="V90" s="53" t="s">
+        <v>150</v>
+      </c>
       <c r="W90" s="53"/>
       <c r="Y90" s="3"/>
-      <c r="Z90" s="3"/>
-      <c r="AG90" s="28"/>
-    </row>
-    <row r="91" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z90" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD90" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG90" s="62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -4950,7 +4965,9 @@
       <c r="E91" s="15"/>
       <c r="F91" s="52"/>
       <c r="G91" s="52"/>
-      <c r="H91" s="58"/>
+      <c r="H91" s="58" t="s">
+        <v>23</v>
+      </c>
       <c r="I91" s="52"/>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
@@ -4964,14 +4981,30 @@
       <c r="S91" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="T91" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="U91" s="8"/>
+      <c r="T91" s="51"/>
+      <c r="U91" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="V91" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="W91" s="53"/>
       <c r="Y91" s="3"/>
-      <c r="AG91" s="28"/>
-    </row>
-    <row r="92" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z91" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD91" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE91" s="3"/>
+      <c r="AF91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG91" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
@@ -4979,30 +5012,41 @@
       <c r="E92" s="15"/>
       <c r="F92" s="52"/>
       <c r="G92" s="52"/>
-      <c r="H92" s="58"/>
-      <c r="I92" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="J92" s="28"/>
-      <c r="K92" s="28"/>
-      <c r="L92" s="28"/>
-      <c r="M92" s="28"/>
-      <c r="N92" s="28"/>
-      <c r="O92" s="28"/>
-      <c r="P92" s="28"/>
-      <c r="Q92" s="28"/>
-      <c r="R92" s="28"/>
-      <c r="S92" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="T92" s="28"/>
-      <c r="U92" s="11" t="s">
-        <v>138</v>
-      </c>
+      <c r="H92" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="15"/>
+      <c r="O92" s="15"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+      <c r="R92" s="15"/>
+      <c r="S92" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="T92" s="15"/>
+      <c r="U92" s="11"/>
+      <c r="V92" s="53"/>
+      <c r="W92" s="53"/>
       <c r="Y92" s="3"/>
-      <c r="AG92" s="28"/>
-    </row>
-    <row r="93" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Z92" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE92" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF92" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG92" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="93" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
@@ -5011,10 +5055,10 @@
       <c r="F93" s="52"/>
       <c r="G93" s="52"/>
       <c r="H93" s="58"/>
-      <c r="I93" s="52"/>
-      <c r="J93" s="52" t="s">
-        <v>38</v>
-      </c>
+      <c r="I93" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="J93" s="15"/>
       <c r="K93" s="15"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
@@ -5026,15 +5070,17 @@
       <c r="S93" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="T93" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="U93" s="8"/>
+      <c r="T93" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="U93" s="11"/>
+      <c r="V93" s="53"/>
+      <c r="W93" s="53"/>
       <c r="Y93" s="3"/>
       <c r="Z93" s="3"/>
       <c r="AG93" s="28"/>
     </row>
-    <row r="94" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="15"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
@@ -5044,10 +5090,8 @@
       <c r="G94" s="52"/>
       <c r="H94" s="58"/>
       <c r="I94" s="52"/>
-      <c r="J94" s="52"/>
-      <c r="K94" s="52" t="s">
-        <v>3</v>
-      </c>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
@@ -5058,30 +5102,14 @@
       <c r="S94" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="T94" s="51"/>
-      <c r="U94" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="V94" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="W94" s="53"/>
+      <c r="T94" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="U94" s="8"/>
       <c r="Y94" s="3"/>
-      <c r="AA94" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD94" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE94" s="3"/>
-      <c r="AF94" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG94" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="95" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG94" s="28"/>
+    </row>
+    <row r="95" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="15"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
@@ -5090,26 +5118,29 @@
       <c r="F95" s="52"/>
       <c r="G95" s="52"/>
       <c r="H95" s="58"/>
-      <c r="I95" s="52"/>
-      <c r="J95" s="52"/>
-      <c r="K95" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L95" s="15"/>
-      <c r="M95" s="15"/>
-      <c r="N95" s="15"/>
-      <c r="O95" s="15"/>
-      <c r="P95" s="15"/>
-      <c r="Q95" s="15"/>
-      <c r="R95" s="15"/>
-      <c r="S95" s="52"/>
-      <c r="T95" s="51"/>
-      <c r="U95" s="8"/>
+      <c r="I95" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="J95" s="28"/>
+      <c r="K95" s="28"/>
+      <c r="L95" s="28"/>
+      <c r="M95" s="28"/>
+      <c r="N95" s="28"/>
+      <c r="O95" s="28"/>
+      <c r="P95" s="28"/>
+      <c r="Q95" s="28"/>
+      <c r="R95" s="28"/>
+      <c r="S95" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="T95" s="28"/>
+      <c r="U95" s="11" t="s">
+        <v>138</v>
+      </c>
       <c r="Y95" s="3"/>
-      <c r="AA95" s="3"/>
       <c r="AG95" s="28"/>
     </row>
-    <row r="96" spans="1:33" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
@@ -5119,40 +5150,29 @@
       <c r="G96" s="52"/>
       <c r="H96" s="58"/>
       <c r="I96" s="52"/>
-      <c r="J96" s="52"/>
+      <c r="J96" s="52" t="s">
+        <v>38</v>
+      </c>
       <c r="K96" s="15"/>
-      <c r="L96" s="52" t="s">
-        <v>34</v>
-      </c>
+      <c r="L96" s="15"/>
       <c r="M96" s="15"/>
       <c r="N96" s="15"/>
       <c r="O96" s="15"/>
       <c r="P96" s="15"/>
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
-      <c r="S96" s="52"/>
-      <c r="T96" s="51"/>
+      <c r="S96" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="T96" s="51" t="s">
+        <v>149</v>
+      </c>
       <c r="U96" s="8"/>
-      <c r="V96" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="W96" s="53"/>
       <c r="Y96" s="3"/>
-      <c r="AA96" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="AD96" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE96" s="3"/>
-      <c r="AF96" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG96" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="97" spans="1:52" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z96" s="3"/>
+      <c r="AG96" s="28"/>
+    </row>
+    <row r="97" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
@@ -5163,35 +5183,43 @@
       <c r="H97" s="58"/>
       <c r="I97" s="52"/>
       <c r="J97" s="52"/>
-      <c r="K97" s="15"/>
-      <c r="L97" s="52"/>
+      <c r="K97" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="L97" s="15"/>
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
       <c r="O97" s="15"/>
       <c r="P97" s="15"/>
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
-      <c r="S97" s="52"/>
+      <c r="S97" s="52" t="s">
+        <v>1</v>
+      </c>
       <c r="T97" s="51"/>
-      <c r="U97" s="8"/>
-      <c r="V97" s="53"/>
+      <c r="U97" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="V97" s="53" t="s">
+        <v>140</v>
+      </c>
       <c r="W97" s="53"/>
       <c r="Y97" s="3"/>
       <c r="AA97" s="3" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="AD97" s="3" t="s">
-        <v>177</v>
+        <v>102</v>
       </c>
       <c r="AE97" s="3"/>
       <c r="AF97" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG97" s="28" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="98" spans="1:52" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -5202,8 +5230,10 @@
       <c r="H98" s="58"/>
       <c r="I98" s="52"/>
       <c r="J98" s="52"/>
-      <c r="K98" s="15"/>
-      <c r="L98" s="52"/>
+      <c r="K98" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L98" s="15"/>
       <c r="M98" s="15"/>
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
@@ -5213,22 +5243,9 @@
       <c r="S98" s="52"/>
       <c r="T98" s="51"/>
       <c r="U98" s="8"/>
-      <c r="V98" s="53"/>
-      <c r="W98" s="53"/>
       <c r="Y98" s="3"/>
-      <c r="AA98" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="AD98" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE98" s="3"/>
-      <c r="AF98" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG98" s="28" t="s">
-        <v>226</v>
-      </c>
+      <c r="AA98" s="3"/>
+      <c r="AG98" s="28"/>
     </row>
     <row r="99" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
@@ -5243,7 +5260,7 @@
       <c r="J99" s="52"/>
       <c r="K99" s="15"/>
       <c r="L99" s="52" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="M99" s="15"/>
       <c r="N99" s="15"/>
@@ -5255,25 +5272,25 @@
       <c r="T99" s="51"/>
       <c r="U99" s="8"/>
       <c r="V99" s="53" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="W99" s="53"/>
       <c r="Y99" s="3"/>
       <c r="AA99" s="3" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="AD99" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AE99" s="3"/>
       <c r="AF99" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG99" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="100" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="100" spans="1:52" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
@@ -5285,9 +5302,7 @@
       <c r="I100" s="52"/>
       <c r="J100" s="52"/>
       <c r="K100" s="15"/>
-      <c r="L100" s="52" t="s">
-        <v>44</v>
-      </c>
+      <c r="L100" s="52"/>
       <c r="M100" s="15"/>
       <c r="N100" s="15"/>
       <c r="O100" s="15"/>
@@ -5296,26 +5311,25 @@
       <c r="R100" s="15"/>
       <c r="S100" s="52"/>
       <c r="T100" s="51"/>
-      <c r="U100" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="V100" s="53" t="s">
-        <v>147</v>
-      </c>
+      <c r="U100" s="8"/>
+      <c r="V100" s="53"/>
       <c r="W100" s="53"/>
       <c r="Y100" s="3"/>
       <c r="AA100" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AD100" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AE100" s="3"/>
+      <c r="AF100" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="AG100" s="28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="101" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="101" spans="1:52" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -5327,7 +5341,7 @@
       <c r="I101" s="52"/>
       <c r="J101" s="52"/>
       <c r="K101" s="15"/>
-      <c r="L101" s="15"/>
+      <c r="L101" s="52"/>
       <c r="M101" s="15"/>
       <c r="N101" s="15"/>
       <c r="O101" s="15"/>
@@ -5337,71 +5351,107 @@
       <c r="S101" s="52"/>
       <c r="T101" s="51"/>
       <c r="U101" s="8"/>
+      <c r="V101" s="53"/>
+      <c r="W101" s="53"/>
       <c r="Y101" s="3"/>
-      <c r="Z101" s="25"/>
-      <c r="AG101" s="28"/>
-    </row>
-    <row r="102" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA101" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD101" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE101" s="3"/>
+      <c r="AF101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG101" s="28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="102" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
-      <c r="B102" s="28"/>
+      <c r="B102" s="15"/>
       <c r="C102" s="15"/>
       <c r="D102" s="15"/>
       <c r="E102" s="15"/>
-      <c r="F102" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G102" s="15"/>
-      <c r="H102" s="15"/>
-      <c r="I102" s="15"/>
-      <c r="J102" s="15"/>
+      <c r="F102" s="52"/>
+      <c r="G102" s="52"/>
+      <c r="H102" s="58"/>
+      <c r="I102" s="52"/>
+      <c r="J102" s="52"/>
       <c r="K102" s="15"/>
-      <c r="L102" s="15"/>
+      <c r="L102" s="52" t="s">
+        <v>45</v>
+      </c>
       <c r="M102" s="15"/>
       <c r="N102" s="15"/>
       <c r="O102" s="15"/>
       <c r="P102" s="15"/>
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
-      <c r="S102" s="52" t="s">
+      <c r="S102" s="52"/>
+      <c r="T102" s="51"/>
+      <c r="U102" s="8"/>
+      <c r="V102" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="W102" s="53"/>
+      <c r="Y102" s="3"/>
+      <c r="AA102" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD102" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T102" s="15"/>
-      <c r="U102" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="V102" s="52"/>
-      <c r="W102" s="52"/>
-      <c r="AG102" s="28"/>
-    </row>
-    <row r="103" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG102" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:52" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H103" s="15"/>
-      <c r="I103" s="15"/>
-      <c r="J103" s="15"/>
+      <c r="F103" s="52"/>
+      <c r="G103" s="52"/>
+      <c r="H103" s="58"/>
+      <c r="I103" s="52"/>
+      <c r="J103" s="52"/>
       <c r="K103" s="15"/>
-      <c r="L103" s="15"/>
+      <c r="L103" s="52" t="s">
+        <v>44</v>
+      </c>
       <c r="M103" s="15"/>
       <c r="N103" s="15"/>
       <c r="O103" s="15"/>
       <c r="P103" s="15"/>
       <c r="Q103" s="15"/>
       <c r="R103" s="15"/>
-      <c r="S103" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T103" s="15"/>
-      <c r="U103" s="10"/>
-      <c r="V103" s="15"/>
-      <c r="W103" s="15"/>
-      <c r="AG103" s="28"/>
+      <c r="S103" s="52"/>
+      <c r="T103" s="51"/>
+      <c r="U103" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="V103" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="W103" s="53"/>
+      <c r="Y103" s="3"/>
+      <c r="AA103" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD103" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE103" s="3"/>
+      <c r="AG103" s="28" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="104" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
@@ -5409,13 +5459,11 @@
       <c r="C104" s="15"/>
       <c r="D104" s="15"/>
       <c r="E104" s="15"/>
-      <c r="F104" s="15"/>
-      <c r="G104" s="15"/>
-      <c r="H104" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I104" s="15"/>
-      <c r="J104" s="15"/>
+      <c r="F104" s="52"/>
+      <c r="G104" s="52"/>
+      <c r="H104" s="58"/>
+      <c r="I104" s="52"/>
+      <c r="J104" s="52"/>
       <c r="K104" s="15"/>
       <c r="L104" s="15"/>
       <c r="M104" s="15"/>
@@ -5424,26 +5472,24 @@
       <c r="P104" s="15"/>
       <c r="Q104" s="15"/>
       <c r="R104" s="15"/>
-      <c r="S104" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="T104" s="15"/>
-      <c r="U104" s="10"/>
-      <c r="V104" s="15"/>
-      <c r="W104" s="15"/>
+      <c r="S104" s="52"/>
+      <c r="T104" s="51"/>
+      <c r="U104" s="8"/>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="25"/>
       <c r="AG104" s="28"/>
     </row>
     <row r="105" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="15"/>
-      <c r="B105" s="15"/>
+      <c r="B105" s="28"/>
       <c r="C105" s="15"/>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
+      <c r="F105" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="G105" s="15"/>
-      <c r="H105" s="15" t="s">
-        <v>40</v>
-      </c>
+      <c r="H105" s="15"/>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
       <c r="K105" s="15"/>
@@ -5454,13 +5500,15 @@
       <c r="P105" s="15"/>
       <c r="Q105" s="15"/>
       <c r="R105" s="15"/>
-      <c r="S105" s="15" t="s">
-        <v>1</v>
+      <c r="S105" s="52" t="s">
+        <v>2</v>
       </c>
       <c r="T105" s="15"/>
-      <c r="U105" s="12"/>
-      <c r="V105" s="54"/>
-      <c r="W105" s="54"/>
+      <c r="U105" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="V105" s="52"/>
+      <c r="W105" s="52"/>
       <c r="AG105" s="28"/>
     </row>
     <row r="106" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5470,10 +5518,10 @@
       <c r="D106" s="15"/>
       <c r="E106" s="15"/>
       <c r="F106" s="15"/>
-      <c r="G106" s="15"/>
-      <c r="H106" s="58" t="s">
-        <v>108</v>
-      </c>
+      <c r="G106" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H106" s="15"/>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
       <c r="K106" s="15"/>
@@ -5484,59 +5532,44 @@
       <c r="P106" s="15"/>
       <c r="Q106" s="15"/>
       <c r="R106" s="15"/>
-      <c r="S106" s="58" t="s">
+      <c r="S106" s="15" t="s">
         <v>1</v>
       </c>
       <c r="T106" s="15"/>
-      <c r="U106" s="12"/>
+      <c r="U106" s="10"/>
+      <c r="V106" s="15"/>
+      <c r="W106" s="15"/>
       <c r="AG106" s="28"/>
     </row>
-    <row r="107" spans="1:52" s="2" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="15"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
       <c r="D107" s="15"/>
       <c r="E107" s="15"/>
       <c r="F107" s="15"/>
-      <c r="G107" s="52"/>
-      <c r="H107" s="15"/>
-      <c r="I107" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I107" s="15"/>
       <c r="J107" s="15"/>
       <c r="K107" s="15"/>
       <c r="L107" s="15"/>
       <c r="M107" s="15"/>
-      <c r="N107" s="28"/>
-      <c r="O107" s="28"/>
+      <c r="N107" s="15"/>
+      <c r="O107" s="15"/>
       <c r="P107" s="15"/>
       <c r="Q107" s="15"/>
       <c r="R107" s="15"/>
       <c r="S107" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T107" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="U107" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="V107" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="W107" s="54"/>
-      <c r="Z107" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="AD107" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF107" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG107" s="53" t="s">
-        <v>152</v>
-      </c>
+      <c r="T107" s="15"/>
+      <c r="U107" s="10"/>
+      <c r="V107" s="15"/>
+      <c r="W107" s="15"/>
+      <c r="AG107" s="28"/>
     </row>
     <row r="108" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
@@ -5546,74 +5579,68 @@
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
       <c r="G108" s="15"/>
-      <c r="H108" s="52"/>
-      <c r="I108" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="H108" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I108" s="15"/>
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
       <c r="L108" s="15"/>
       <c r="M108" s="15"/>
-      <c r="N108" s="28"/>
-      <c r="O108" s="28"/>
+      <c r="N108" s="15"/>
+      <c r="O108" s="15"/>
       <c r="P108" s="15"/>
       <c r="Q108" s="15"/>
       <c r="R108" s="15"/>
       <c r="S108" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="T108" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="U108" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="V108" s="38"/>
-      <c r="W108" s="38"/>
+      <c r="T108" s="15"/>
+      <c r="U108" s="12"/>
+      <c r="V108" s="54"/>
+      <c r="W108" s="54"/>
       <c r="AG108" s="28"/>
-      <c r="AZ108" s="2" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="109" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
-      <c r="B109" s="28"/>
+      <c r="B109" s="15"/>
       <c r="C109" s="15"/>
       <c r="D109" s="15"/>
       <c r="E109" s="15"/>
       <c r="F109" s="15"/>
       <c r="G109" s="15"/>
-      <c r="H109" s="52"/>
-      <c r="I109" s="52"/>
+      <c r="H109" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="I109" s="15"/>
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
       <c r="L109" s="15"/>
       <c r="M109" s="15"/>
-      <c r="N109" s="28"/>
-      <c r="O109" s="28"/>
+      <c r="N109" s="15"/>
+      <c r="O109" s="15"/>
       <c r="P109" s="15"/>
       <c r="Q109" s="15"/>
       <c r="R109" s="15"/>
-      <c r="S109" s="58"/>
-      <c r="T109" s="52"/>
-      <c r="U109" s="19"/>
-      <c r="V109" s="55"/>
-      <c r="W109" s="55"/>
+      <c r="S109" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="T109" s="15"/>
+      <c r="U109" s="12"/>
       <c r="AG109" s="28"/>
-      <c r="AZ109" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="110" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:52" s="2" customFormat="1" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A110" s="15"/>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
       <c r="E110" s="15"/>
       <c r="F110" s="15"/>
-      <c r="G110" s="15"/>
+      <c r="G110" s="52"/>
       <c r="H110" s="15"/>
-      <c r="I110" s="15"/>
+      <c r="I110" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
       <c r="L110" s="15"/>
@@ -5623,28 +5650,44 @@
       <c r="P110" s="15"/>
       <c r="Q110" s="15"/>
       <c r="R110" s="15"/>
-      <c r="S110" s="15"/>
-      <c r="T110" s="15"/>
-      <c r="U110" s="19"/>
-      <c r="V110" s="55"/>
-      <c r="W110" s="55"/>
-      <c r="AG110" s="28"/>
-      <c r="AZ110" s="2" t="s">
-        <v>87</v>
+      <c r="S110" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T110" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="U110" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="V110" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="W110" s="54"/>
+      <c r="Z110" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD110" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF110" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG110" s="53" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
-      <c r="B111" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
       <c r="E111" s="15"/>
       <c r="F111" s="15"/>
       <c r="G111" s="15"/>
-      <c r="H111" s="15"/>
-      <c r="I111" s="15"/>
+      <c r="H111" s="52"/>
+      <c r="I111" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="J111" s="15"/>
       <c r="K111" s="15"/>
       <c r="L111" s="15"/>
@@ -5654,26 +5697,32 @@
       <c r="P111" s="15"/>
       <c r="Q111" s="15"/>
       <c r="R111" s="15"/>
-      <c r="S111" s="15"/>
-      <c r="T111" s="28"/>
-      <c r="U111" s="19"/>
-      <c r="V111" s="55"/>
-      <c r="W111" s="55"/>
+      <c r="S111" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T111" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="U111" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="V111" s="38"/>
+      <c r="W111" s="38"/>
       <c r="AG111" s="28"/>
       <c r="AZ111" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="28"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15"/>
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
       <c r="G112" s="15"/>
-      <c r="H112" s="15"/>
-      <c r="I112" s="15"/>
+      <c r="H112" s="52"/>
+      <c r="I112" s="52"/>
       <c r="J112" s="15"/>
       <c r="K112" s="15"/>
       <c r="L112" s="15"/>
@@ -5683,25 +5732,25 @@
       <c r="P112" s="15"/>
       <c r="Q112" s="15"/>
       <c r="R112" s="15"/>
-      <c r="S112" s="15"/>
-      <c r="T112" s="15"/>
-      <c r="U112" s="8"/>
-      <c r="V112" s="28"/>
-      <c r="W112" s="28"/>
+      <c r="S112" s="58"/>
+      <c r="T112" s="52"/>
+      <c r="U112" s="19"/>
+      <c r="V112" s="55"/>
+      <c r="W112" s="55"/>
       <c r="AG112" s="28"/>
       <c r="AZ112" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="113" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="15"/>
-      <c r="B113" s="15"/>
-      <c r="C113" s="15"/>
-      <c r="D113" s="15"/>
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
       <c r="E113" s="15"/>
-      <c r="F113" s="28"/>
-      <c r="G113" s="28"/>
-      <c r="H113" s="52"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="15"/>
+      <c r="H113" s="15"/>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
       <c r="K113" s="15"/>
@@ -5714,21 +5763,26 @@
       <c r="R113" s="15"/>
       <c r="S113" s="15"/>
       <c r="T113" s="15"/>
-      <c r="U113" s="12"/>
-      <c r="V113" s="54"/>
-      <c r="W113" s="54"/>
+      <c r="U113" s="19"/>
+      <c r="V113" s="55"/>
+      <c r="W113" s="55"/>
       <c r="AG113" s="28"/>
-    </row>
-    <row r="114" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AZ113" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="114" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="15"/>
-      <c r="D114" s="15"/>
+      <c r="B114" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
       <c r="E114" s="15"/>
-      <c r="F114" s="28"/>
-      <c r="G114" s="28"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
       <c r="H114" s="15"/>
-      <c r="I114" s="52"/>
+      <c r="I114" s="15"/>
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
       <c r="L114" s="15"/>
@@ -5739,22 +5793,25 @@
       <c r="Q114" s="15"/>
       <c r="R114" s="15"/>
       <c r="S114" s="15"/>
-      <c r="T114" s="52"/>
-      <c r="U114" s="12"/>
-      <c r="V114" s="54"/>
-      <c r="W114" s="54"/>
+      <c r="T114" s="28"/>
+      <c r="U114" s="19"/>
+      <c r="V114" s="55"/>
+      <c r="W114" s="55"/>
       <c r="AG114" s="28"/>
-    </row>
-    <row r="115" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AZ114" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="115" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="15"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
+      <c r="B115" s="28"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
       <c r="E115" s="15"/>
-      <c r="F115" s="28"/>
-      <c r="G115" s="28"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
       <c r="H115" s="15"/>
-      <c r="I115" s="52"/>
+      <c r="I115" s="15"/>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
       <c r="L115" s="15"/>
@@ -5765,13 +5822,16 @@
       <c r="Q115" s="15"/>
       <c r="R115" s="15"/>
       <c r="S115" s="15"/>
-      <c r="T115" s="28"/>
-      <c r="U115" s="10"/>
-      <c r="V115" s="15"/>
-      <c r="W115" s="15"/>
+      <c r="T115" s="15"/>
+      <c r="U115" s="8"/>
+      <c r="V115" s="28"/>
+      <c r="W115" s="28"/>
       <c r="AG115" s="28"/>
-    </row>
-    <row r="116" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AZ115" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
       <c r="C116" s="15"/>
@@ -5779,8 +5839,8 @@
       <c r="E116" s="15"/>
       <c r="F116" s="28"/>
       <c r="G116" s="28"/>
-      <c r="H116" s="15"/>
-      <c r="I116" s="52"/>
+      <c r="H116" s="52"/>
+      <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
       <c r="L116" s="15"/>
@@ -5791,13 +5851,13 @@
       <c r="Q116" s="15"/>
       <c r="R116" s="15"/>
       <c r="S116" s="15"/>
-      <c r="T116" s="28"/>
-      <c r="U116" s="52"/>
-      <c r="V116" s="52"/>
-      <c r="W116" s="52"/>
+      <c r="T116" s="15"/>
+      <c r="U116" s="12"/>
+      <c r="V116" s="54"/>
+      <c r="W116" s="54"/>
       <c r="AG116" s="28"/>
     </row>
-    <row r="117" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="15"/>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
@@ -5817,22 +5877,22 @@
       <c r="Q117" s="15"/>
       <c r="R117" s="15"/>
       <c r="S117" s="15"/>
-      <c r="T117" s="51"/>
-      <c r="U117" s="52"/>
-      <c r="V117" s="52"/>
-      <c r="W117" s="52"/>
+      <c r="T117" s="52"/>
+      <c r="U117" s="12"/>
+      <c r="V117" s="54"/>
+      <c r="W117" s="54"/>
       <c r="AG117" s="28"/>
     </row>
-    <row r="118" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="15"/>
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
-      <c r="F118" s="15"/>
-      <c r="G118" s="15"/>
-      <c r="H118" s="52"/>
-      <c r="I118" s="15"/>
+      <c r="F118" s="28"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="52"/>
       <c r="J118" s="15"/>
       <c r="K118" s="15"/>
       <c r="L118" s="15"/>
@@ -5843,124 +5903,124 @@
       <c r="Q118" s="15"/>
       <c r="R118" s="15"/>
       <c r="S118" s="15"/>
-      <c r="T118" s="15"/>
-      <c r="U118" s="54"/>
-      <c r="V118" s="54"/>
-      <c r="W118" s="54"/>
+      <c r="T118" s="28"/>
+      <c r="U118" s="10"/>
+      <c r="V118" s="15"/>
+      <c r="W118" s="15"/>
       <c r="AG118" s="28"/>
     </row>
-    <row r="119" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="15"/>
       <c r="B119" s="15"/>
       <c r="C119" s="15"/>
       <c r="D119" s="15"/>
       <c r="E119" s="15"/>
-      <c r="F119" s="15"/>
-      <c r="G119" s="15"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="28"/>
       <c r="H119" s="15"/>
-      <c r="I119" s="15"/>
+      <c r="I119" s="52"/>
       <c r="J119" s="15"/>
       <c r="K119" s="15"/>
       <c r="L119" s="15"/>
       <c r="M119" s="15"/>
-      <c r="N119" s="15"/>
-      <c r="O119" s="15"/>
+      <c r="N119" s="28"/>
+      <c r="O119" s="28"/>
       <c r="P119" s="15"/>
       <c r="Q119" s="15"/>
       <c r="R119" s="15"/>
       <c r="S119" s="15"/>
-      <c r="T119" s="15"/>
-      <c r="U119" s="15"/>
-      <c r="V119" s="15"/>
-      <c r="W119" s="15"/>
+      <c r="T119" s="28"/>
+      <c r="U119" s="52"/>
+      <c r="V119" s="52"/>
+      <c r="W119" s="52"/>
       <c r="AG119" s="28"/>
     </row>
-    <row r="120" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
-      <c r="I120" s="4"/>
-      <c r="J120" s="4"/>
-      <c r="K120" s="4"/>
-      <c r="L120" s="4"/>
-      <c r="M120" s="4"/>
-      <c r="N120" s="4"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-      <c r="Q120" s="4"/>
-      <c r="R120" s="4"/>
-      <c r="S120" s="4"/>
-      <c r="T120" s="4"/>
-      <c r="U120" s="15"/>
-      <c r="V120" s="15"/>
-      <c r="W120" s="15"/>
+    <row r="120" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="15"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="15"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="28"/>
+      <c r="G120" s="28"/>
+      <c r="H120" s="15"/>
+      <c r="I120" s="52"/>
+      <c r="J120" s="15"/>
+      <c r="K120" s="15"/>
+      <c r="L120" s="15"/>
+      <c r="M120" s="15"/>
+      <c r="N120" s="28"/>
+      <c r="O120" s="28"/>
+      <c r="P120" s="15"/>
+      <c r="Q120" s="15"/>
+      <c r="R120" s="15"/>
+      <c r="S120" s="15"/>
+      <c r="T120" s="51"/>
+      <c r="U120" s="52"/>
+      <c r="V120" s="52"/>
+      <c r="W120" s="52"/>
       <c r="AG120" s="28"/>
     </row>
-    <row r="121" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
-      <c r="I121" s="4"/>
-      <c r="J121" s="4"/>
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="M121" s="4"/>
-      <c r="N121" s="4"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-      <c r="Q121" s="4"/>
-      <c r="R121" s="4"/>
-      <c r="S121" s="4"/>
-      <c r="T121" s="4"/>
-      <c r="U121" s="15"/>
-      <c r="V121" s="15"/>
-      <c r="W121" s="15"/>
+    <row r="121" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="15"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="15"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="52"/>
+      <c r="I121" s="15"/>
+      <c r="J121" s="15"/>
+      <c r="K121" s="15"/>
+      <c r="L121" s="15"/>
+      <c r="M121" s="15"/>
+      <c r="N121" s="28"/>
+      <c r="O121" s="28"/>
+      <c r="P121" s="15"/>
+      <c r="Q121" s="15"/>
+      <c r="R121" s="15"/>
+      <c r="S121" s="15"/>
+      <c r="T121" s="15"/>
+      <c r="U121" s="54"/>
+      <c r="V121" s="54"/>
+      <c r="W121" s="54"/>
       <c r="AG121" s="28"/>
     </row>
-    <row r="122" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="4"/>
-      <c r="J122" s="4"/>
-      <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-      <c r="M122" s="4"/>
-      <c r="N122" s="4"/>
-      <c r="O122" s="4"/>
-      <c r="P122" s="4"/>
-      <c r="Q122" s="4"/>
-      <c r="R122" s="4"/>
-      <c r="S122" s="4"/>
-      <c r="T122" s="4"/>
+    <row r="122" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="15"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15"/>
+      <c r="H122" s="15"/>
+      <c r="I122" s="15"/>
+      <c r="J122" s="15"/>
+      <c r="K122" s="15"/>
+      <c r="L122" s="15"/>
+      <c r="M122" s="15"/>
+      <c r="N122" s="15"/>
+      <c r="O122" s="15"/>
+      <c r="P122" s="15"/>
+      <c r="Q122" s="15"/>
+      <c r="R122" s="15"/>
+      <c r="S122" s="15"/>
+      <c r="T122" s="15"/>
       <c r="U122" s="15"/>
       <c r="V122" s="15"/>
       <c r="W122" s="15"/>
       <c r="AG122" s="28"/>
     </row>
-    <row r="123" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
-      <c r="G123" s="5"/>
+      <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
@@ -5971,12 +6031,15 @@
       <c r="O123" s="4"/>
       <c r="P123" s="4"/>
       <c r="Q123" s="4"/>
+      <c r="R123" s="4"/>
+      <c r="S123" s="4"/>
       <c r="T123" s="4"/>
-      <c r="U123" s="28"/>
-      <c r="V123" s="28"/>
-      <c r="W123" s="28"/>
-    </row>
-    <row r="124" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U123" s="15"/>
+      <c r="V123" s="15"/>
+      <c r="W123" s="15"/>
+      <c r="AG123" s="28"/>
+    </row>
+    <row r="124" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -5984,7 +6047,7 @@
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
       <c r="G124" s="4"/>
-      <c r="H124" s="5"/>
+      <c r="H124" s="4"/>
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
       <c r="K124" s="4"/>
@@ -5994,12 +6057,15 @@
       <c r="O124" s="4"/>
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
+      <c r="R124" s="4"/>
+      <c r="S124" s="4"/>
       <c r="T124" s="4"/>
       <c r="U124" s="15"/>
       <c r="V124" s="15"/>
       <c r="W124" s="15"/>
-    </row>
-    <row r="125" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG124" s="28"/>
+    </row>
+    <row r="125" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -6007,7 +6073,7 @@
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
-      <c r="H125" s="5"/>
+      <c r="H125" s="4"/>
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
       <c r="K125" s="4"/>
@@ -6017,20 +6083,23 @@
       <c r="O125" s="4"/>
       <c r="P125" s="4"/>
       <c r="Q125" s="4"/>
+      <c r="R125" s="4"/>
+      <c r="S125" s="4"/>
       <c r="T125" s="4"/>
       <c r="U125" s="15"/>
       <c r="V125" s="15"/>
       <c r="W125" s="15"/>
-    </row>
-    <row r="126" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AG125" s="28"/>
+    </row>
+    <row r="126" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
-      <c r="G126" s="4"/>
-      <c r="H126" s="5"/>
+      <c r="G126" s="5"/>
+      <c r="H126" s="4"/>
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
@@ -6041,11 +6110,11 @@
       <c r="P126" s="4"/>
       <c r="Q126" s="4"/>
       <c r="T126" s="4"/>
-      <c r="U126" s="15"/>
-      <c r="V126" s="15"/>
-      <c r="W126" s="15"/>
-    </row>
-    <row r="127" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U126" s="28"/>
+      <c r="V126" s="28"/>
+      <c r="W126" s="28"/>
+    </row>
+    <row r="127" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -6053,8 +6122,8 @@
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
-      <c r="H127" s="4"/>
-      <c r="I127" s="5"/>
+      <c r="H127" s="5"/>
+      <c r="I127" s="4"/>
       <c r="J127" s="4"/>
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
@@ -6068,7 +6137,7 @@
       <c r="V127" s="15"/>
       <c r="W127" s="15"/>
     </row>
-    <row r="128" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -6076,8 +6145,8 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
-      <c r="I128" s="5"/>
+      <c r="H128" s="5"/>
+      <c r="I128" s="4"/>
       <c r="J128" s="4"/>
       <c r="K128" s="4"/>
       <c r="L128" s="4"/>
@@ -6087,9 +6156,9 @@
       <c r="P128" s="4"/>
       <c r="Q128" s="4"/>
       <c r="T128" s="4"/>
-      <c r="U128" s="52"/>
-      <c r="V128" s="52"/>
-      <c r="W128" s="52"/>
+      <c r="U128" s="15"/>
+      <c r="V128" s="15"/>
+      <c r="W128" s="15"/>
     </row>
     <row r="129" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
@@ -6110,11 +6179,11 @@
       <c r="P129" s="4"/>
       <c r="Q129" s="4"/>
       <c r="T129" s="4"/>
-      <c r="U129" s="54"/>
-      <c r="V129" s="54"/>
-      <c r="W129" s="54"/>
-    </row>
-    <row r="130" spans="1:23" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U129" s="15"/>
+      <c r="V129" s="15"/>
+      <c r="W129" s="15"/>
+    </row>
+    <row r="130" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -6133,9 +6202,9 @@
       <c r="P130" s="4"/>
       <c r="Q130" s="4"/>
       <c r="T130" s="4"/>
-      <c r="U130" s="54"/>
-      <c r="V130" s="54"/>
-      <c r="W130" s="54"/>
+      <c r="U130" s="15"/>
+      <c r="V130" s="15"/>
+      <c r="W130" s="15"/>
     </row>
     <row r="131" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
@@ -6155,9 +6224,10 @@
       <c r="O131" s="4"/>
       <c r="P131" s="4"/>
       <c r="Q131" s="4"/>
-      <c r="U131" s="15"/>
-      <c r="V131" s="15"/>
-      <c r="W131" s="15"/>
+      <c r="T131" s="4"/>
+      <c r="U131" s="52"/>
+      <c r="V131" s="52"/>
+      <c r="W131" s="52"/>
     </row>
     <row r="132" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
@@ -6165,8 +6235,10 @@
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="5"/>
+      <c r="F132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="4"/>
       <c r="J132" s="4"/>
       <c r="K132" s="4"/>
       <c r="L132" s="4"/>
@@ -6175,12 +6247,12 @@
       <c r="O132" s="4"/>
       <c r="P132" s="4"/>
       <c r="Q132" s="4"/>
-      <c r="T132" s="5"/>
-      <c r="U132" s="52"/>
-      <c r="V132" s="52"/>
-      <c r="W132" s="52"/>
-    </row>
-    <row r="133" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="T132" s="4"/>
+      <c r="U132" s="54"/>
+      <c r="V132" s="54"/>
+      <c r="W132" s="54"/>
+    </row>
+    <row r="133" spans="1:23" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6199,9 +6271,9 @@
       <c r="P133" s="4"/>
       <c r="Q133" s="4"/>
       <c r="T133" s="4"/>
-      <c r="U133" s="52"/>
-      <c r="V133" s="52"/>
-      <c r="W133" s="52"/>
+      <c r="U133" s="54"/>
+      <c r="V133" s="54"/>
+      <c r="W133" s="54"/>
     </row>
     <row r="134" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
@@ -6211,8 +6283,8 @@
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
-      <c r="H134" s="5"/>
-      <c r="I134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="5"/>
       <c r="J134" s="4"/>
       <c r="K134" s="4"/>
       <c r="L134" s="4"/>
@@ -6221,35 +6293,86 @@
       <c r="O134" s="4"/>
       <c r="P134" s="4"/>
       <c r="Q134" s="4"/>
-      <c r="S134" s="4"/>
-      <c r="T134" s="4"/>
-      <c r="U134" s="54"/>
-      <c r="V134" s="54"/>
-      <c r="W134" s="54"/>
+      <c r="U134" s="15"/>
+      <c r="V134" s="15"/>
+      <c r="W134" s="15"/>
     </row>
     <row r="135" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I135" s="3"/>
-      <c r="U135" s="28"/>
-      <c r="V135" s="28"/>
-      <c r="W135" s="28"/>
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="4"/>
+      <c r="E135" s="4"/>
+      <c r="H135" s="4"/>
+      <c r="I135" s="5"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4"/>
+      <c r="T135" s="5"/>
+      <c r="U135" s="52"/>
+      <c r="V135" s="52"/>
+      <c r="W135" s="52"/>
     </row>
     <row r="136" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J136" s="3"/>
-      <c r="U136" s="28"/>
-      <c r="V136" s="28"/>
-      <c r="W136" s="28"/>
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="4"/>
+      <c r="G136" s="4"/>
+      <c r="H136" s="4"/>
+      <c r="I136" s="5"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+      <c r="N136" s="4"/>
+      <c r="O136" s="4"/>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4"/>
+      <c r="T136" s="4"/>
+      <c r="U136" s="52"/>
+      <c r="V136" s="52"/>
+      <c r="W136" s="52"/>
     </row>
     <row r="137" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="U137" s="28"/>
-      <c r="V137" s="28"/>
-      <c r="W137" s="28"/>
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" s="4"/>
+      <c r="F137" s="4"/>
+      <c r="G137" s="4"/>
+      <c r="H137" s="5"/>
+      <c r="I137" s="4"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="4"/>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+      <c r="N137" s="4"/>
+      <c r="O137" s="4"/>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4"/>
+      <c r="S137" s="4"/>
+      <c r="T137" s="4"/>
+      <c r="U137" s="54"/>
+      <c r="V137" s="54"/>
+      <c r="W137" s="54"/>
     </row>
     <row r="138" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I138" s="3"/>
       <c r="U138" s="28"/>
       <c r="V138" s="28"/>
       <c r="W138" s="28"/>
     </row>
     <row r="139" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J139" s="3"/>
       <c r="U139" s="28"/>
       <c r="V139" s="28"/>
       <c r="W139" s="28"/>
@@ -6313,6 +6436,21 @@
       <c r="U151" s="28"/>
       <c r="V151" s="28"/>
       <c r="W151" s="28"/>
+    </row>
+    <row r="152" spans="21:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U152" s="28"/>
+      <c r="V152" s="28"/>
+      <c r="W152" s="28"/>
+    </row>
+    <row r="153" spans="21:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U153" s="28"/>
+      <c r="V153" s="28"/>
+      <c r="W153" s="28"/>
+    </row>
+    <row r="154" spans="21:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U154" s="28"/>
+      <c r="V154" s="28"/>
+      <c r="W154" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Uppdaterat kardinalitet för accountableHealthcareProfessional
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/clinicalprocess/logistics/logistics/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontakt.xlsx
+++ b/ServiceInteractions/riv/clinicalprocess/logistics/logistics/trunk/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Vård- och omsorgskontakt.xlsx
@@ -10,7 +10,7 @@
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
     <sheet name="Blad1" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -547,7 +547,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -687,6 +687,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1037,8 +1038,8 @@
   <dimension ref="A1:V99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1202,7 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="26"/>
       <c r="B9" s="26"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="53" t="s">
         <v>60</v>
       </c>
       <c r="D9" s="3"/>
@@ -1334,7 +1335,7 @@
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="24" t="s">
         <v>110</v>

</xml_diff>